<commit_message>
adicion nombre producto a la exportacion de datos etiquetas
</commit_message>
<xml_diff>
--- a/html/etiquetas/etiquetasDispensacion.xlsx
+++ b/html/etiquetas/etiquetasDispensacion.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="6">
   <si>
     <t>Orden</t>
   </si>
@@ -26,7 +26,13 @@
     <t>Peso</t>
   </si>
   <si>
+    <t>Producto</t>
+  </si>
+  <si>
     <t>OP001/21</t>
+  </si>
+  <si>
+    <t>jabon liquido - mawie (500 ml)</t>
   </si>
 </sst>
 </file>
@@ -365,7 +371,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -373,7 +379,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -383,10 +389,13 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2">
         <v>10005</v>
@@ -394,10 +403,13 @@
       <c r="C2">
         <v>9.2</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B3">
         <v>10007</v>
@@ -405,10 +417,13 @@
       <c r="C3">
         <v>12.88</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B4">
         <v>10012</v>
@@ -416,10 +431,13 @@
       <c r="C4">
         <v>14.72</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="D4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5">
         <v>10011</v>
@@ -427,16 +445,22 @@
       <c r="C5">
         <v>23.92</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
+      <c r="D5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>10003</v>
       </c>
       <c r="C6">
         <v>0.92</v>
+      </c>
+      <c r="D6" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>